<commit_message>
added documentation notes, added UID field, cleaned up file names
</commit_message>
<xml_diff>
--- a/Department data page.xlsx
+++ b/Department data page.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/panda/Desktop/Automate forms project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FE429CF-0054-5F47-85D3-1373FF8C427F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D499EB0-CE83-1C48-9794-E708ADA4722F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8760" yWindow="460" windowWidth="28040" windowHeight="14780" xr2:uid="{41EDBBFD-3744-2546-BBF5-46C0335A03A4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>First year of AY</t>
   </si>
@@ -33,9 +33,6 @@
     <t>base_salary</t>
   </si>
   <si>
-    <t>Range adjustment percentage</t>
-  </si>
-  <si>
     <t>Dept code</t>
   </si>
   <si>
@@ -58,6 +55,15 @@
   </si>
   <si>
     <t>Mathletes</t>
+  </si>
+  <si>
+    <t>Dept Approver</t>
+  </si>
+  <si>
+    <t>Ms. Norbury, Mathletes Coach</t>
+  </si>
+  <si>
+    <t>Range adjustment percentage eff 7/1</t>
   </si>
 </sst>
 </file>
@@ -409,15 +415,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49A90F19-6612-E146-9316-7BC7B67F7BFB}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.83203125" customWidth="1"/>
+    <col min="1" max="1" width="31.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -438,7 +444,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -446,7 +452,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>4444</v>
@@ -454,15 +460,15 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>45678</v>
@@ -470,18 +476,26 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
         <v>9</v>
       </c>
-      <c r="B8" t="s">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>